<commit_message>
Finished bar introduction and BOM
</commit_message>
<xml_diff>
--- a/Documentation/Gantt Chart.xlsx
+++ b/Documentation/Gantt Chart.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D247A8-36A8-4F14-8190-AACBD61AB281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC6D8D6-7BDE-452A-9F18-802039BC2995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
   <si>
     <t>Create a Project Schedule in this worksheet.
 Enter title of this project in cell B1. 
@@ -1194,7 +1194,7 @@
     <xf numFmtId="0" fontId="9" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1402,61 +1402,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="45" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="3" xfId="9" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="47" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="5" fillId="47" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1466,17 +1411,8 @@
     <xf numFmtId="166" fontId="5" fillId="47" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="47" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="9" fillId="47" borderId="2" xfId="10" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="47" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="47" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1552,6 +1488,73 @@
     </xf>
     <xf numFmtId="166" fontId="9" fillId="46" borderId="2" xfId="10" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="3" xfId="9" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="45" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="47" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="47" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="47" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -2252,9 +2255,9 @@
   </sheetPr>
   <dimension ref="A1:KQ61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F42" sqref="F42:F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2300,445 +2303,445 @@
       <c r="B3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="113" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="82"/>
-      <c r="E3" s="84">
+      <c r="D3" s="114"/>
+      <c r="E3" s="116">
         <v>44440</v>
       </c>
-      <c r="F3" s="84"/>
+      <c r="F3" s="116"/>
     </row>
     <row r="4" spans="1:303" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="82"/>
+      <c r="D4" s="114"/>
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="78">
+      <c r="I4" s="102">
         <f>I5</f>
         <v>44438</v>
       </c>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="79"/>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="78">
+      <c r="J4" s="103"/>
+      <c r="K4" s="103"/>
+      <c r="L4" s="103"/>
+      <c r="M4" s="103"/>
+      <c r="N4" s="103"/>
+      <c r="O4" s="109"/>
+      <c r="P4" s="102">
         <f>P5</f>
         <v>44445</v>
       </c>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="79"/>
-      <c r="S4" s="79"/>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="78">
+      <c r="Q4" s="103"/>
+      <c r="R4" s="103"/>
+      <c r="S4" s="103"/>
+      <c r="T4" s="103"/>
+      <c r="U4" s="103"/>
+      <c r="V4" s="109"/>
+      <c r="W4" s="102">
         <f>W5</f>
         <v>44452</v>
       </c>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="79"/>
-      <c r="Z4" s="79"/>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="90"/>
-      <c r="AD4" s="78">
+      <c r="X4" s="103"/>
+      <c r="Y4" s="103"/>
+      <c r="Z4" s="103"/>
+      <c r="AA4" s="103"/>
+      <c r="AB4" s="103"/>
+      <c r="AC4" s="109"/>
+      <c r="AD4" s="102">
         <f>AD5</f>
         <v>44459</v>
       </c>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="79"/>
-      <c r="AG4" s="79"/>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="90"/>
-      <c r="AK4" s="78">
+      <c r="AE4" s="103"/>
+      <c r="AF4" s="103"/>
+      <c r="AG4" s="103"/>
+      <c r="AH4" s="103"/>
+      <c r="AI4" s="103"/>
+      <c r="AJ4" s="109"/>
+      <c r="AK4" s="102">
         <f>AK5</f>
         <v>44466</v>
       </c>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="79"/>
-      <c r="AN4" s="79"/>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="90"/>
-      <c r="AR4" s="78">
+      <c r="AL4" s="103"/>
+      <c r="AM4" s="103"/>
+      <c r="AN4" s="103"/>
+      <c r="AO4" s="103"/>
+      <c r="AP4" s="103"/>
+      <c r="AQ4" s="109"/>
+      <c r="AR4" s="102">
         <f>AR5</f>
         <v>44473</v>
       </c>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="79"/>
-      <c r="AU4" s="79"/>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="90"/>
-      <c r="AY4" s="78">
+      <c r="AS4" s="103"/>
+      <c r="AT4" s="103"/>
+      <c r="AU4" s="103"/>
+      <c r="AV4" s="103"/>
+      <c r="AW4" s="103"/>
+      <c r="AX4" s="109"/>
+      <c r="AY4" s="102">
         <f>AY5</f>
         <v>44480</v>
       </c>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="79"/>
-      <c r="BB4" s="79"/>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="90"/>
-      <c r="BF4" s="78">
+      <c r="AZ4" s="103"/>
+      <c r="BA4" s="103"/>
+      <c r="BB4" s="103"/>
+      <c r="BC4" s="103"/>
+      <c r="BD4" s="103"/>
+      <c r="BE4" s="109"/>
+      <c r="BF4" s="102">
         <f>BF5</f>
         <v>44487</v>
       </c>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="79"/>
-      <c r="BI4" s="79"/>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="79"/>
-      <c r="BM4" s="78">
+      <c r="BG4" s="103"/>
+      <c r="BH4" s="103"/>
+      <c r="BI4" s="103"/>
+      <c r="BJ4" s="103"/>
+      <c r="BK4" s="103"/>
+      <c r="BL4" s="103"/>
+      <c r="BM4" s="102">
         <f>BM5</f>
         <v>44494</v>
       </c>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="79"/>
-      <c r="BP4" s="79"/>
-      <c r="BQ4" s="79"/>
-      <c r="BR4" s="79"/>
-      <c r="BS4" s="79"/>
-      <c r="BT4" s="78">
+      <c r="BN4" s="103"/>
+      <c r="BO4" s="103"/>
+      <c r="BP4" s="103"/>
+      <c r="BQ4" s="103"/>
+      <c r="BR4" s="103"/>
+      <c r="BS4" s="103"/>
+      <c r="BT4" s="102">
         <f>BT5</f>
         <v>44501</v>
       </c>
-      <c r="BU4" s="79"/>
-      <c r="BV4" s="79"/>
-      <c r="BW4" s="79"/>
-      <c r="BX4" s="79"/>
-      <c r="BY4" s="79"/>
-      <c r="BZ4" s="79"/>
-      <c r="CA4" s="78">
+      <c r="BU4" s="103"/>
+      <c r="BV4" s="103"/>
+      <c r="BW4" s="103"/>
+      <c r="BX4" s="103"/>
+      <c r="BY4" s="103"/>
+      <c r="BZ4" s="103"/>
+      <c r="CA4" s="102">
         <f t="shared" ref="CA4" si="0">CA5</f>
         <v>44508</v>
       </c>
-      <c r="CB4" s="79"/>
-      <c r="CC4" s="79"/>
-      <c r="CD4" s="79"/>
-      <c r="CE4" s="79"/>
-      <c r="CF4" s="79"/>
-      <c r="CG4" s="79"/>
-      <c r="CH4" s="78">
+      <c r="CB4" s="103"/>
+      <c r="CC4" s="103"/>
+      <c r="CD4" s="103"/>
+      <c r="CE4" s="103"/>
+      <c r="CF4" s="103"/>
+      <c r="CG4" s="103"/>
+      <c r="CH4" s="102">
         <f t="shared" ref="CH4" si="1">CH5</f>
         <v>44515</v>
       </c>
-      <c r="CI4" s="79"/>
-      <c r="CJ4" s="79"/>
-      <c r="CK4" s="79"/>
-      <c r="CL4" s="79"/>
-      <c r="CM4" s="79"/>
-      <c r="CN4" s="79"/>
-      <c r="CO4" s="78">
+      <c r="CI4" s="103"/>
+      <c r="CJ4" s="103"/>
+      <c r="CK4" s="103"/>
+      <c r="CL4" s="103"/>
+      <c r="CM4" s="103"/>
+      <c r="CN4" s="103"/>
+      <c r="CO4" s="102">
         <f t="shared" ref="CO4" si="2">CO5</f>
         <v>44522</v>
       </c>
-      <c r="CP4" s="79"/>
-      <c r="CQ4" s="79"/>
-      <c r="CR4" s="79"/>
-      <c r="CS4" s="79"/>
-      <c r="CT4" s="79"/>
-      <c r="CU4" s="79"/>
-      <c r="CV4" s="78">
+      <c r="CP4" s="103"/>
+      <c r="CQ4" s="103"/>
+      <c r="CR4" s="103"/>
+      <c r="CS4" s="103"/>
+      <c r="CT4" s="103"/>
+      <c r="CU4" s="103"/>
+      <c r="CV4" s="102">
         <f t="shared" ref="CV4" si="3">CV5</f>
         <v>44529</v>
       </c>
-      <c r="CW4" s="79"/>
-      <c r="CX4" s="79"/>
-      <c r="CY4" s="79"/>
-      <c r="CZ4" s="79"/>
-      <c r="DA4" s="79"/>
-      <c r="DB4" s="79"/>
-      <c r="DC4" s="78">
+      <c r="CW4" s="103"/>
+      <c r="CX4" s="103"/>
+      <c r="CY4" s="103"/>
+      <c r="CZ4" s="103"/>
+      <c r="DA4" s="103"/>
+      <c r="DB4" s="103"/>
+      <c r="DC4" s="102">
         <f>DC5</f>
         <v>44536</v>
       </c>
-      <c r="DD4" s="79"/>
-      <c r="DE4" s="79"/>
-      <c r="DF4" s="79"/>
-      <c r="DG4" s="79"/>
-      <c r="DH4" s="79"/>
-      <c r="DI4" s="79"/>
-      <c r="DJ4" s="78">
+      <c r="DD4" s="103"/>
+      <c r="DE4" s="103"/>
+      <c r="DF4" s="103"/>
+      <c r="DG4" s="103"/>
+      <c r="DH4" s="103"/>
+      <c r="DI4" s="103"/>
+      <c r="DJ4" s="102">
         <f t="shared" ref="DJ4" si="4">DJ5</f>
         <v>44543</v>
       </c>
-      <c r="DK4" s="79"/>
-      <c r="DL4" s="79"/>
-      <c r="DM4" s="79"/>
-      <c r="DN4" s="79"/>
-      <c r="DO4" s="79"/>
-      <c r="DP4" s="79"/>
-      <c r="DQ4" s="78">
+      <c r="DK4" s="103"/>
+      <c r="DL4" s="103"/>
+      <c r="DM4" s="103"/>
+      <c r="DN4" s="103"/>
+      <c r="DO4" s="103"/>
+      <c r="DP4" s="103"/>
+      <c r="DQ4" s="102">
         <f t="shared" ref="DQ4" si="5">DQ5</f>
         <v>44550</v>
       </c>
-      <c r="DR4" s="79"/>
-      <c r="DS4" s="79"/>
-      <c r="DT4" s="79"/>
-      <c r="DU4" s="79"/>
-      <c r="DV4" s="79"/>
-      <c r="DW4" s="79"/>
-      <c r="DX4" s="78">
+      <c r="DR4" s="103"/>
+      <c r="DS4" s="103"/>
+      <c r="DT4" s="103"/>
+      <c r="DU4" s="103"/>
+      <c r="DV4" s="103"/>
+      <c r="DW4" s="103"/>
+      <c r="DX4" s="102">
         <f t="shared" ref="DX4" si="6">DX5</f>
         <v>44557</v>
       </c>
-      <c r="DY4" s="79"/>
-      <c r="DZ4" s="79"/>
-      <c r="EA4" s="79"/>
-      <c r="EB4" s="79"/>
-      <c r="EC4" s="79"/>
-      <c r="ED4" s="79"/>
-      <c r="EE4" s="78">
+      <c r="DY4" s="103"/>
+      <c r="DZ4" s="103"/>
+      <c r="EA4" s="103"/>
+      <c r="EB4" s="103"/>
+      <c r="EC4" s="103"/>
+      <c r="ED4" s="103"/>
+      <c r="EE4" s="102">
         <f t="shared" ref="EE4" si="7">EE5</f>
         <v>44564</v>
       </c>
-      <c r="EF4" s="79"/>
-      <c r="EG4" s="79"/>
-      <c r="EH4" s="79"/>
-      <c r="EI4" s="79"/>
-      <c r="EJ4" s="79"/>
-      <c r="EK4" s="79"/>
-      <c r="EL4" s="78">
+      <c r="EF4" s="103"/>
+      <c r="EG4" s="103"/>
+      <c r="EH4" s="103"/>
+      <c r="EI4" s="103"/>
+      <c r="EJ4" s="103"/>
+      <c r="EK4" s="103"/>
+      <c r="EL4" s="102">
         <f t="shared" ref="EL4" si="8">EL5</f>
         <v>44571</v>
       </c>
-      <c r="EM4" s="79"/>
-      <c r="EN4" s="79"/>
-      <c r="EO4" s="79"/>
-      <c r="EP4" s="79"/>
-      <c r="EQ4" s="79"/>
-      <c r="ER4" s="79"/>
-      <c r="ES4" s="78">
+      <c r="EM4" s="103"/>
+      <c r="EN4" s="103"/>
+      <c r="EO4" s="103"/>
+      <c r="EP4" s="103"/>
+      <c r="EQ4" s="103"/>
+      <c r="ER4" s="103"/>
+      <c r="ES4" s="102">
         <f t="shared" ref="ES4" si="9">ES5</f>
         <v>44578</v>
       </c>
-      <c r="ET4" s="79"/>
-      <c r="EU4" s="79"/>
-      <c r="EV4" s="79"/>
-      <c r="EW4" s="79"/>
-      <c r="EX4" s="79"/>
-      <c r="EY4" s="79"/>
-      <c r="EZ4" s="78">
+      <c r="ET4" s="103"/>
+      <c r="EU4" s="103"/>
+      <c r="EV4" s="103"/>
+      <c r="EW4" s="103"/>
+      <c r="EX4" s="103"/>
+      <c r="EY4" s="103"/>
+      <c r="EZ4" s="102">
         <f t="shared" ref="EZ4" si="10">EZ5</f>
         <v>44585</v>
       </c>
-      <c r="FA4" s="79"/>
-      <c r="FB4" s="79"/>
-      <c r="FC4" s="79"/>
-      <c r="FD4" s="79"/>
-      <c r="FE4" s="79"/>
-      <c r="FF4" s="79"/>
-      <c r="FG4" s="78">
+      <c r="FA4" s="103"/>
+      <c r="FB4" s="103"/>
+      <c r="FC4" s="103"/>
+      <c r="FD4" s="103"/>
+      <c r="FE4" s="103"/>
+      <c r="FF4" s="103"/>
+      <c r="FG4" s="102">
         <f t="shared" ref="FG4" si="11">FG5</f>
         <v>44592</v>
       </c>
-      <c r="FH4" s="79"/>
-      <c r="FI4" s="79"/>
-      <c r="FJ4" s="79"/>
-      <c r="FK4" s="79"/>
-      <c r="FL4" s="79"/>
-      <c r="FM4" s="79"/>
-      <c r="FN4" s="78">
+      <c r="FH4" s="103"/>
+      <c r="FI4" s="103"/>
+      <c r="FJ4" s="103"/>
+      <c r="FK4" s="103"/>
+      <c r="FL4" s="103"/>
+      <c r="FM4" s="103"/>
+      <c r="FN4" s="102">
         <f t="shared" ref="FN4" si="12">FN5</f>
         <v>44599</v>
       </c>
-      <c r="FO4" s="79"/>
-      <c r="FP4" s="79"/>
-      <c r="FQ4" s="79"/>
-      <c r="FR4" s="79"/>
-      <c r="FS4" s="79"/>
-      <c r="FT4" s="79"/>
-      <c r="FU4" s="78">
+      <c r="FO4" s="103"/>
+      <c r="FP4" s="103"/>
+      <c r="FQ4" s="103"/>
+      <c r="FR4" s="103"/>
+      <c r="FS4" s="103"/>
+      <c r="FT4" s="103"/>
+      <c r="FU4" s="102">
         <f t="shared" ref="FU4" si="13">FU5</f>
         <v>44606</v>
       </c>
-      <c r="FV4" s="79"/>
-      <c r="FW4" s="79"/>
-      <c r="FX4" s="79"/>
-      <c r="FY4" s="79"/>
-      <c r="FZ4" s="79"/>
-      <c r="GA4" s="79"/>
-      <c r="GB4" s="78">
+      <c r="FV4" s="103"/>
+      <c r="FW4" s="103"/>
+      <c r="FX4" s="103"/>
+      <c r="FY4" s="103"/>
+      <c r="FZ4" s="103"/>
+      <c r="GA4" s="103"/>
+      <c r="GB4" s="102">
         <f t="shared" ref="GB4" si="14">GB5</f>
         <v>44613</v>
       </c>
-      <c r="GC4" s="79"/>
-      <c r="GD4" s="79"/>
-      <c r="GE4" s="79"/>
-      <c r="GF4" s="79"/>
-      <c r="GG4" s="79"/>
-      <c r="GH4" s="79"/>
-      <c r="GI4" s="78">
+      <c r="GC4" s="103"/>
+      <c r="GD4" s="103"/>
+      <c r="GE4" s="103"/>
+      <c r="GF4" s="103"/>
+      <c r="GG4" s="103"/>
+      <c r="GH4" s="103"/>
+      <c r="GI4" s="102">
         <f t="shared" ref="GI4" si="15">GI5</f>
         <v>44620</v>
       </c>
-      <c r="GJ4" s="79"/>
-      <c r="GK4" s="79"/>
-      <c r="GL4" s="79"/>
-      <c r="GM4" s="79"/>
-      <c r="GN4" s="79"/>
-      <c r="GO4" s="79"/>
-      <c r="GP4" s="78">
+      <c r="GJ4" s="103"/>
+      <c r="GK4" s="103"/>
+      <c r="GL4" s="103"/>
+      <c r="GM4" s="103"/>
+      <c r="GN4" s="103"/>
+      <c r="GO4" s="103"/>
+      <c r="GP4" s="102">
         <f t="shared" ref="GP4" si="16">GP5</f>
         <v>44627</v>
       </c>
-      <c r="GQ4" s="79"/>
-      <c r="GR4" s="79"/>
-      <c r="GS4" s="79"/>
-      <c r="GT4" s="79"/>
-      <c r="GU4" s="79"/>
-      <c r="GV4" s="79"/>
-      <c r="GW4" s="78">
+      <c r="GQ4" s="103"/>
+      <c r="GR4" s="103"/>
+      <c r="GS4" s="103"/>
+      <c r="GT4" s="103"/>
+      <c r="GU4" s="103"/>
+      <c r="GV4" s="103"/>
+      <c r="GW4" s="102">
         <f t="shared" ref="GW4" si="17">GW5</f>
         <v>44634</v>
       </c>
-      <c r="GX4" s="79"/>
-      <c r="GY4" s="79"/>
-      <c r="GZ4" s="79"/>
-      <c r="HA4" s="79"/>
-      <c r="HB4" s="79"/>
-      <c r="HC4" s="79"/>
-      <c r="HD4" s="78">
+      <c r="GX4" s="103"/>
+      <c r="GY4" s="103"/>
+      <c r="GZ4" s="103"/>
+      <c r="HA4" s="103"/>
+      <c r="HB4" s="103"/>
+      <c r="HC4" s="103"/>
+      <c r="HD4" s="102">
         <f t="shared" ref="HD4" si="18">HD5</f>
         <v>44641</v>
       </c>
-      <c r="HE4" s="79"/>
-      <c r="HF4" s="79"/>
-      <c r="HG4" s="79"/>
-      <c r="HH4" s="79"/>
-      <c r="HI4" s="79"/>
-      <c r="HJ4" s="79"/>
-      <c r="HK4" s="78">
+      <c r="HE4" s="103"/>
+      <c r="HF4" s="103"/>
+      <c r="HG4" s="103"/>
+      <c r="HH4" s="103"/>
+      <c r="HI4" s="103"/>
+      <c r="HJ4" s="103"/>
+      <c r="HK4" s="102">
         <f t="shared" ref="HK4" si="19">HK5</f>
         <v>44648</v>
       </c>
-      <c r="HL4" s="79"/>
-      <c r="HM4" s="79"/>
-      <c r="HN4" s="79"/>
-      <c r="HO4" s="79"/>
-      <c r="HP4" s="79"/>
-      <c r="HQ4" s="79"/>
-      <c r="HR4" s="78">
+      <c r="HL4" s="103"/>
+      <c r="HM4" s="103"/>
+      <c r="HN4" s="103"/>
+      <c r="HO4" s="103"/>
+      <c r="HP4" s="103"/>
+      <c r="HQ4" s="103"/>
+      <c r="HR4" s="102">
         <f t="shared" ref="HR4" si="20">HR5</f>
         <v>44655</v>
       </c>
-      <c r="HS4" s="79"/>
-      <c r="HT4" s="79"/>
-      <c r="HU4" s="79"/>
-      <c r="HV4" s="79"/>
-      <c r="HW4" s="79"/>
-      <c r="HX4" s="79"/>
-      <c r="HY4" s="78">
+      <c r="HS4" s="103"/>
+      <c r="HT4" s="103"/>
+      <c r="HU4" s="103"/>
+      <c r="HV4" s="103"/>
+      <c r="HW4" s="103"/>
+      <c r="HX4" s="103"/>
+      <c r="HY4" s="102">
         <f t="shared" ref="HY4" si="21">HY5</f>
         <v>44662</v>
       </c>
-      <c r="HZ4" s="79"/>
-      <c r="IA4" s="79"/>
-      <c r="IB4" s="79"/>
-      <c r="IC4" s="79"/>
-      <c r="ID4" s="79"/>
-      <c r="IE4" s="79"/>
-      <c r="IF4" s="78">
+      <c r="HZ4" s="103"/>
+      <c r="IA4" s="103"/>
+      <c r="IB4" s="103"/>
+      <c r="IC4" s="103"/>
+      <c r="ID4" s="103"/>
+      <c r="IE4" s="103"/>
+      <c r="IF4" s="102">
         <f t="shared" ref="IF4" si="22">IF5</f>
         <v>44669</v>
       </c>
-      <c r="IG4" s="79"/>
-      <c r="IH4" s="79"/>
-      <c r="II4" s="79"/>
-      <c r="IJ4" s="79"/>
-      <c r="IK4" s="79"/>
-      <c r="IL4" s="79"/>
-      <c r="IM4" s="78">
+      <c r="IG4" s="103"/>
+      <c r="IH4" s="103"/>
+      <c r="II4" s="103"/>
+      <c r="IJ4" s="103"/>
+      <c r="IK4" s="103"/>
+      <c r="IL4" s="103"/>
+      <c r="IM4" s="102">
         <f t="shared" ref="IM4" si="23">IM5</f>
         <v>44676</v>
       </c>
-      <c r="IN4" s="79"/>
-      <c r="IO4" s="79"/>
-      <c r="IP4" s="79"/>
-      <c r="IQ4" s="79"/>
-      <c r="IR4" s="79"/>
-      <c r="IS4" s="79"/>
-      <c r="IT4" s="78">
+      <c r="IN4" s="103"/>
+      <c r="IO4" s="103"/>
+      <c r="IP4" s="103"/>
+      <c r="IQ4" s="103"/>
+      <c r="IR4" s="103"/>
+      <c r="IS4" s="103"/>
+      <c r="IT4" s="102">
         <f t="shared" ref="IT4" si="24">IT5</f>
         <v>44683</v>
       </c>
-      <c r="IU4" s="79"/>
-      <c r="IV4" s="79"/>
-      <c r="IW4" s="79"/>
-      <c r="IX4" s="79"/>
-      <c r="IY4" s="79"/>
-      <c r="IZ4" s="79"/>
-      <c r="JA4" s="78">
+      <c r="IU4" s="103"/>
+      <c r="IV4" s="103"/>
+      <c r="IW4" s="103"/>
+      <c r="IX4" s="103"/>
+      <c r="IY4" s="103"/>
+      <c r="IZ4" s="103"/>
+      <c r="JA4" s="102">
         <f t="shared" ref="JA4" si="25">JA5</f>
         <v>44690</v>
       </c>
-      <c r="JB4" s="79"/>
-      <c r="JC4" s="79"/>
-      <c r="JD4" s="79"/>
-      <c r="JE4" s="79"/>
-      <c r="JF4" s="79"/>
-      <c r="JG4" s="79"/>
-      <c r="JH4" s="78">
+      <c r="JB4" s="103"/>
+      <c r="JC4" s="103"/>
+      <c r="JD4" s="103"/>
+      <c r="JE4" s="103"/>
+      <c r="JF4" s="103"/>
+      <c r="JG4" s="103"/>
+      <c r="JH4" s="102">
         <f t="shared" ref="JH4" si="26">JH5</f>
         <v>44697</v>
       </c>
-      <c r="JI4" s="79"/>
-      <c r="JJ4" s="79"/>
-      <c r="JK4" s="79"/>
-      <c r="JL4" s="79"/>
-      <c r="JM4" s="79"/>
-      <c r="JN4" s="79"/>
-      <c r="JO4" s="76"/>
-      <c r="JP4" s="76"/>
-      <c r="JQ4" s="76"/>
-      <c r="JR4" s="76"/>
-      <c r="JS4" s="76"/>
-      <c r="JT4" s="76"/>
-      <c r="JU4" s="76"/>
-      <c r="JV4" s="76"/>
-      <c r="JW4" s="76"/>
-      <c r="JX4" s="76"/>
-      <c r="JY4" s="76"/>
-      <c r="JZ4" s="76"/>
-      <c r="KA4" s="76"/>
-      <c r="KB4" s="76"/>
-      <c r="KC4" s="76"/>
-      <c r="KD4" s="76"/>
-      <c r="KE4" s="76"/>
-      <c r="KF4" s="76"/>
-      <c r="KG4" s="76"/>
-      <c r="KH4" s="76"/>
-      <c r="KI4" s="76"/>
-      <c r="KJ4" s="76"/>
-      <c r="KK4" s="76"/>
-      <c r="KL4" s="76"/>
-      <c r="KM4" s="76"/>
-      <c r="KN4" s="76"/>
-      <c r="KO4" s="76"/>
-      <c r="KP4" s="76"/>
+      <c r="JI4" s="103"/>
+      <c r="JJ4" s="103"/>
+      <c r="JK4" s="103"/>
+      <c r="JL4" s="103"/>
+      <c r="JM4" s="103"/>
+      <c r="JN4" s="103"/>
+      <c r="JO4" s="119"/>
+      <c r="JP4" s="119"/>
+      <c r="JQ4" s="119"/>
+      <c r="JR4" s="119"/>
+      <c r="JS4" s="119"/>
+      <c r="JT4" s="119"/>
+      <c r="JU4" s="119"/>
+      <c r="JV4" s="119"/>
+      <c r="JW4" s="119"/>
+      <c r="JX4" s="119"/>
+      <c r="JY4" s="119"/>
+      <c r="JZ4" s="119"/>
+      <c r="KA4" s="119"/>
+      <c r="KB4" s="119"/>
+      <c r="KC4" s="119"/>
+      <c r="KD4" s="119"/>
+      <c r="KE4" s="119"/>
+      <c r="KF4" s="119"/>
+      <c r="KG4" s="119"/>
+      <c r="KH4" s="119"/>
+      <c r="KI4" s="119"/>
+      <c r="KJ4" s="119"/>
+      <c r="KK4" s="119"/>
+      <c r="KL4" s="119"/>
+      <c r="KM4" s="119"/>
+      <c r="KN4" s="119"/>
+      <c r="KO4" s="119"/>
+      <c r="KP4" s="119"/>
     </row>
     <row r="5" spans="1:303" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
+      <c r="B5" s="115"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
       <c r="I5" s="65">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44438</v>
@@ -3837,10 +3840,10 @@
       <c r="A6" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="88"/>
+      <c r="C6" s="105"/>
       <c r="D6" s="61" t="s">
         <v>11</v>
       </c>
@@ -5018,10 +5021,10 @@
       <c r="A8" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="89" t="s">
+      <c r="B8" s="106" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="74"/>
+      <c r="C8" s="107"/>
       <c r="D8" s="11"/>
       <c r="E8" s="46"/>
       <c r="F8" s="47"/>
@@ -5301,10 +5304,10 @@
       <c r="A9" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="85" t="s">
+      <c r="B9" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="74"/>
+      <c r="C9" s="107"/>
       <c r="D9" s="12">
         <v>1</v>
       </c>
@@ -5591,10 +5594,10 @@
       <c r="A10" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="74"/>
+      <c r="C10" s="107"/>
       <c r="D10" s="12">
         <v>1</v>
       </c>
@@ -5878,10 +5881,10 @@
     </row>
     <row r="11" spans="1:303" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="37"/>
-      <c r="B11" s="85" t="s">
+      <c r="B11" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="74"/>
+      <c r="C11" s="107"/>
       <c r="D11" s="12">
         <v>1</v>
       </c>
@@ -6166,10 +6169,10 @@
     </row>
     <row r="12" spans="1:303" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="37"/>
-      <c r="B12" s="85" t="s">
+      <c r="B12" s="108" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="74"/>
+      <c r="C12" s="107"/>
       <c r="D12" s="12">
         <v>1</v>
       </c>
@@ -6456,10 +6459,10 @@
       <c r="A13" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="86" t="s">
+      <c r="B13" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="80"/>
+      <c r="C13" s="112"/>
       <c r="D13" s="13"/>
       <c r="E13" s="48"/>
       <c r="F13" s="49"/>
@@ -6737,10 +6740,10 @@
     </row>
     <row r="14" spans="1:303" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="38"/>
-      <c r="B14" s="77" t="s">
+      <c r="B14" s="110" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="74"/>
+      <c r="C14" s="107"/>
       <c r="D14" s="14">
         <v>1</v>
       </c>
@@ -7025,10 +7028,10 @@
     </row>
     <row r="15" spans="1:303" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="37"/>
-      <c r="B15" s="77" t="s">
+      <c r="B15" s="110" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="74"/>
+      <c r="C15" s="107"/>
       <c r="D15" s="14">
         <v>1</v>
       </c>
@@ -7313,10 +7316,10 @@
     </row>
     <row r="16" spans="1:303" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="37"/>
-      <c r="B16" s="77" t="s">
+      <c r="B16" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="74"/>
+      <c r="C16" s="107"/>
       <c r="D16" s="14">
         <v>1</v>
       </c>
@@ -7602,10 +7605,10 @@
     </row>
     <row r="17" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="37"/>
-      <c r="B17" s="77" t="s">
+      <c r="B17" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="74"/>
+      <c r="C17" s="107"/>
       <c r="D17" s="14">
         <v>1</v>
       </c>
@@ -7891,10 +7894,10 @@
     </row>
     <row r="18" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="37"/>
-      <c r="B18" s="77" t="s">
+      <c r="B18" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="74"/>
+      <c r="C18" s="107"/>
       <c r="D18" s="14">
         <v>1</v>
       </c>
@@ -8177,10 +8180,10 @@
     </row>
     <row r="19" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="37"/>
-      <c r="B19" s="77" t="s">
+      <c r="B19" s="110" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="74"/>
+      <c r="C19" s="107"/>
       <c r="D19" s="14">
         <v>1</v>
       </c>
@@ -8465,10 +8468,10 @@
     </row>
     <row r="20" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37"/>
-      <c r="B20" s="77" t="s">
+      <c r="B20" s="110" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="74"/>
+      <c r="C20" s="107"/>
       <c r="D20" s="14">
         <v>1</v>
       </c>
@@ -8753,10 +8756,10 @@
       <c r="A21" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="75" t="s">
+      <c r="B21" s="111" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="80"/>
+      <c r="C21" s="112"/>
       <c r="D21" s="15"/>
       <c r="E21" s="50"/>
       <c r="F21" s="51"/>
@@ -9034,10 +9037,10 @@
     </row>
     <row r="22" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="37"/>
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="124" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="74"/>
+      <c r="C22" s="107"/>
       <c r="D22" s="16">
         <v>1</v>
       </c>
@@ -9321,10 +9324,10 @@
     </row>
     <row r="23" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="37"/>
-      <c r="B23" s="73" t="s">
+      <c r="B23" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="74"/>
+      <c r="C23" s="107"/>
       <c r="D23" s="16">
         <v>1</v>
       </c>
@@ -9608,10 +9611,10 @@
     </row>
     <row r="24" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="37"/>
-      <c r="B24" s="73" t="s">
+      <c r="B24" s="118" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="74"/>
+      <c r="C24" s="107"/>
       <c r="D24" s="16">
         <v>1</v>
       </c>
@@ -9895,10 +9898,10 @@
     </row>
     <row r="25" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="37"/>
-      <c r="B25" s="73" t="s">
+      <c r="B25" s="118" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="74"/>
+      <c r="C25" s="107"/>
       <c r="D25" s="16">
         <v>1</v>
       </c>
@@ -10182,12 +10185,12 @@
     </row>
     <row r="26" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="37"/>
-      <c r="B26" s="73" t="s">
+      <c r="B26" s="118" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="74"/>
+      <c r="C26" s="107"/>
       <c r="D26" s="16">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E26" s="58">
         <v>44634</v>
@@ -10469,12 +10472,12 @@
     </row>
     <row r="27" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37"/>
-      <c r="B27" s="73" t="s">
+      <c r="B27" s="118" t="s">
         <v>63</v>
       </c>
-      <c r="C27" s="74"/>
+      <c r="C27" s="107"/>
       <c r="D27" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="58">
         <v>44641</v>
@@ -10758,13 +10761,13 @@
       <c r="A28" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="91" t="s">
+      <c r="B28" s="123" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="91"/>
-      <c r="D28" s="92"/>
-      <c r="E28" s="93"/>
-      <c r="F28" s="94"/>
+      <c r="C28" s="123"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="75"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10" t="str">
         <f t="shared" si="40"/>
@@ -11039,17 +11042,17 @@
     </row>
     <row r="29" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="37"/>
-      <c r="B29" s="95" t="s">
+      <c r="B29" s="120" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="96"/>
-      <c r="D29" s="92">
+      <c r="C29" s="121"/>
+      <c r="D29" s="73">
         <v>1</v>
       </c>
-      <c r="E29" s="97">
+      <c r="E29" s="76">
         <v>44620</v>
       </c>
-      <c r="F29" s="97">
+      <c r="F29" s="76">
         <v>44623</v>
       </c>
       <c r="G29" s="10"/>
@@ -11326,17 +11329,17 @@
     </row>
     <row r="30" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="37"/>
-      <c r="B30" s="95" t="s">
+      <c r="B30" s="120" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="96"/>
-      <c r="D30" s="92">
+      <c r="C30" s="121"/>
+      <c r="D30" s="73">
         <v>1</v>
       </c>
-      <c r="E30" s="97">
+      <c r="E30" s="76">
         <v>44623</v>
       </c>
-      <c r="F30" s="97">
+      <c r="F30" s="76">
         <v>44627</v>
       </c>
       <c r="G30" s="10"/>
@@ -11613,17 +11616,17 @@
     </row>
     <row r="31" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="37"/>
-      <c r="B31" s="95" t="s">
+      <c r="B31" s="120" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="96"/>
-      <c r="D31" s="92">
+      <c r="C31" s="121"/>
+      <c r="D31" s="73">
         <v>1</v>
       </c>
-      <c r="E31" s="97">
+      <c r="E31" s="76">
         <v>44627</v>
       </c>
-      <c r="F31" s="97">
+      <c r="F31" s="76">
         <v>44634</v>
       </c>
       <c r="G31" s="10"/>
@@ -11900,17 +11903,17 @@
     </row>
     <row r="32" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="37"/>
-      <c r="B32" s="98" t="s">
+      <c r="B32" s="122" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="98"/>
-      <c r="D32" s="92">
-        <v>0.5</v>
-      </c>
-      <c r="E32" s="97">
+      <c r="C32" s="122"/>
+      <c r="D32" s="73">
+        <v>1</v>
+      </c>
+      <c r="E32" s="76">
         <v>44634</v>
       </c>
-      <c r="F32" s="97">
+      <c r="F32" s="76">
         <v>44641</v>
       </c>
       <c r="G32" s="10"/>
@@ -12189,17 +12192,17 @@
       <c r="A33" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="99" t="s">
+      <c r="B33" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="99"/>
-      <c r="D33" s="92">
-        <v>0</v>
-      </c>
-      <c r="E33" s="97">
+      <c r="C33" s="77"/>
+      <c r="D33" s="73">
+        <v>1</v>
+      </c>
+      <c r="E33" s="76">
         <v>44641</v>
       </c>
-      <c r="F33" s="97">
+      <c r="F33" s="76">
         <v>44648</v>
       </c>
       <c r="G33" s="10"/>
@@ -12478,17 +12481,17 @@
       <c r="A34" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="99" t="s">
+      <c r="B34" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="99"/>
-      <c r="D34" s="92">
-        <v>0</v>
-      </c>
-      <c r="E34" s="97">
+      <c r="C34" s="77"/>
+      <c r="D34" s="73">
+        <v>1</v>
+      </c>
+      <c r="E34" s="76">
         <v>44648</v>
       </c>
-      <c r="F34" s="97">
+      <c r="F34" s="76">
         <v>44683</v>
       </c>
       <c r="G34" s="10"/>
@@ -12792,13 +12795,13 @@
       <c r="KP34" s="69"/>
     </row>
     <row r="35" spans="1:302" s="3" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="100" t="s">
+      <c r="B35" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="100"/>
-      <c r="D35" s="101"/>
-      <c r="E35" s="102"/>
-      <c r="F35" s="103"/>
+      <c r="C35" s="78"/>
+      <c r="D35" s="79"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="81"/>
       <c r="G35" s="10"/>
       <c r="H35" s="10" t="str">
         <f t="shared" si="40"/>
@@ -13072,17 +13075,17 @@
       <c r="JN35" s="67"/>
     </row>
     <row r="36" spans="1:302" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="104" t="s">
+      <c r="B36" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="104"/>
-      <c r="D36" s="101">
+      <c r="C36" s="82"/>
+      <c r="D36" s="79">
         <v>1</v>
       </c>
-      <c r="E36" s="105">
+      <c r="E36" s="83">
         <v>44522</v>
       </c>
-      <c r="F36" s="105">
+      <c r="F36" s="83">
         <v>44529</v>
       </c>
       <c r="G36" s="10"/>
@@ -13358,17 +13361,17 @@
       <c r="JN36" s="67"/>
     </row>
     <row r="37" spans="1:302" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="104" t="s">
+      <c r="B37" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="C37" s="104"/>
-      <c r="D37" s="101">
+      <c r="C37" s="82"/>
+      <c r="D37" s="79">
         <v>1</v>
       </c>
-      <c r="E37" s="105">
+      <c r="E37" s="83">
         <v>44606</v>
       </c>
-      <c r="F37" s="105">
+      <c r="F37" s="83">
         <v>44608</v>
       </c>
       <c r="G37" s="10"/>
@@ -13644,17 +13647,17 @@
       <c r="JN37" s="67"/>
     </row>
     <row r="38" spans="1:302" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="104" t="s">
+      <c r="B38" s="82" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="104"/>
-      <c r="D38" s="101">
+      <c r="C38" s="82"/>
+      <c r="D38" s="79">
         <v>1</v>
       </c>
-      <c r="E38" s="105">
+      <c r="E38" s="83">
         <v>44627</v>
       </c>
-      <c r="F38" s="105">
+      <c r="F38" s="83">
         <v>44631</v>
       </c>
       <c r="G38" s="10"/>
@@ -13930,17 +13933,17 @@
       <c r="JN38" s="67"/>
     </row>
     <row r="39" spans="1:302" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="104" t="s">
+      <c r="B39" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="104"/>
-      <c r="D39" s="101">
+      <c r="C39" s="82"/>
+      <c r="D39" s="79">
         <v>1</v>
       </c>
-      <c r="E39" s="105">
+      <c r="E39" s="83">
         <v>44631</v>
       </c>
-      <c r="F39" s="105">
+      <c r="F39" s="83">
         <v>44634</v>
       </c>
       <c r="G39" s="10"/>
@@ -14216,17 +14219,17 @@
       <c r="JN39" s="67"/>
     </row>
     <row r="40" spans="1:302" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="104" t="s">
+      <c r="B40" s="82" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="104"/>
-      <c r="D40" s="101">
-        <v>0.8</v>
-      </c>
-      <c r="E40" s="105">
+      <c r="C40" s="82"/>
+      <c r="D40" s="79">
+        <v>1</v>
+      </c>
+      <c r="E40" s="83">
         <v>44613</v>
       </c>
-      <c r="F40" s="105">
+      <c r="F40" s="83">
         <v>44641</v>
       </c>
       <c r="G40" s="10"/>
@@ -14502,13 +14505,13 @@
       <c r="JN40" s="67"/>
     </row>
     <row r="41" spans="1:302" s="3" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="106" t="s">
+      <c r="B41" s="84" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="106"/>
-      <c r="D41" s="107"/>
-      <c r="E41" s="108"/>
-      <c r="F41" s="109"/>
+      <c r="C41" s="84"/>
+      <c r="D41" s="85"/>
+      <c r="E41" s="86"/>
+      <c r="F41" s="87"/>
       <c r="G41" s="10"/>
       <c r="H41" s="10" t="str">
         <f t="shared" si="40"/>
@@ -14782,17 +14785,23 @@
       <c r="JN41" s="67"/>
     </row>
     <row r="42" spans="1:302" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="110" t="s">
+      <c r="B42" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="C42" s="110"/>
-      <c r="D42" s="107"/>
-      <c r="E42" s="111"/>
-      <c r="F42" s="111"/>
+      <c r="C42" s="88"/>
+      <c r="D42" s="85">
+        <v>1</v>
+      </c>
+      <c r="E42" s="89">
+        <v>44627</v>
+      </c>
+      <c r="F42" s="89">
+        <v>44630</v>
+      </c>
       <c r="G42" s="10"/>
-      <c r="H42" s="10" t="str">
+      <c r="H42" s="10">
         <f t="shared" si="40"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="I42" s="23"/>
       <c r="J42" s="23"/>
@@ -15062,17 +15071,23 @@
       <c r="JN42" s="67"/>
     </row>
     <row r="43" spans="1:302" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="110" t="s">
+      <c r="B43" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="110"/>
-      <c r="D43" s="107"/>
-      <c r="E43" s="111"/>
-      <c r="F43" s="111"/>
+      <c r="C43" s="88"/>
+      <c r="D43" s="85">
+        <v>1</v>
+      </c>
+      <c r="E43" s="89">
+        <v>44630</v>
+      </c>
+      <c r="F43" s="89">
+        <v>44641</v>
+      </c>
       <c r="G43" s="10"/>
-      <c r="H43" s="10" t="str">
+      <c r="H43" s="10">
         <f t="shared" si="40"/>
-        <v/>
+        <v>12</v>
       </c>
       <c r="I43" s="23"/>
       <c r="J43" s="23"/>
@@ -15342,17 +15357,23 @@
       <c r="JN43" s="67"/>
     </row>
     <row r="44" spans="1:302" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="110" t="s">
+      <c r="B44" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="110"/>
-      <c r="D44" s="107"/>
-      <c r="E44" s="111"/>
-      <c r="F44" s="111"/>
+      <c r="C44" s="88"/>
+      <c r="D44" s="85">
+        <v>1</v>
+      </c>
+      <c r="E44" s="89">
+        <v>44641</v>
+      </c>
+      <c r="F44" s="89">
+        <v>44648</v>
+      </c>
       <c r="G44" s="10"/>
-      <c r="H44" s="10" t="str">
+      <c r="H44" s="10">
         <f t="shared" si="40"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="I44" s="23"/>
       <c r="J44" s="23"/>
@@ -15622,17 +15643,23 @@
       <c r="JN44" s="67"/>
     </row>
     <row r="45" spans="1:302" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="110" t="s">
+      <c r="B45" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="110"/>
-      <c r="D45" s="107"/>
-      <c r="E45" s="111"/>
-      <c r="F45" s="111"/>
+      <c r="C45" s="88"/>
+      <c r="D45" s="85">
+        <v>1</v>
+      </c>
+      <c r="E45" s="89">
+        <v>44648</v>
+      </c>
+      <c r="F45" s="89">
+        <v>44676</v>
+      </c>
       <c r="G45" s="10"/>
-      <c r="H45" s="10" t="str">
+      <c r="H45" s="10">
         <f t="shared" si="40"/>
-        <v/>
+        <v>29</v>
       </c>
       <c r="I45" s="23"/>
       <c r="J45" s="23"/>
@@ -15902,17 +15929,23 @@
       <c r="JN45" s="67"/>
     </row>
     <row r="46" spans="1:302" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="110" t="s">
+      <c r="B46" s="88" t="s">
         <v>63</v>
       </c>
-      <c r="C46" s="110"/>
-      <c r="D46" s="107"/>
-      <c r="E46" s="111"/>
-      <c r="F46" s="111"/>
+      <c r="C46" s="88"/>
+      <c r="D46" s="85">
+        <v>1</v>
+      </c>
+      <c r="E46" s="89">
+        <v>44676</v>
+      </c>
+      <c r="F46" s="89">
+        <v>44690</v>
+      </c>
       <c r="G46" s="10"/>
-      <c r="H46" s="10" t="str">
+      <c r="H46" s="10">
         <f t="shared" si="40"/>
-        <v/>
+        <v>15</v>
       </c>
       <c r="I46" s="23"/>
       <c r="J46" s="23"/>
@@ -16182,13 +16215,13 @@
       <c r="JN46" s="67"/>
     </row>
     <row r="47" spans="1:302" s="3" customFormat="1" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="112" t="s">
+      <c r="B47" s="90" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="112"/>
-      <c r="D47" s="113"/>
-      <c r="E47" s="114"/>
-      <c r="F47" s="115"/>
+      <c r="C47" s="90"/>
+      <c r="D47" s="91"/>
+      <c r="E47" s="92"/>
+      <c r="F47" s="93"/>
       <c r="G47" s="10"/>
       <c r="H47" s="10" t="str">
         <f t="shared" si="40"/>
@@ -16462,17 +16495,23 @@
       <c r="JN47" s="67"/>
     </row>
     <row r="48" spans="1:302" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="116" t="s">
+      <c r="B48" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="C48" s="116"/>
-      <c r="D48" s="113"/>
-      <c r="E48" s="117"/>
-      <c r="F48" s="117"/>
+      <c r="C48" s="94"/>
+      <c r="D48" s="91">
+        <v>1</v>
+      </c>
+      <c r="E48" s="95">
+        <v>44627</v>
+      </c>
+      <c r="F48" s="95">
+        <v>44630</v>
+      </c>
       <c r="G48" s="10"/>
-      <c r="H48" s="10" t="str">
+      <c r="H48" s="10">
         <f t="shared" si="40"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="I48" s="23"/>
       <c r="J48" s="23"/>
@@ -16742,17 +16781,23 @@
       <c r="JN48" s="67"/>
     </row>
     <row r="49" spans="2:274" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="116" t="s">
+      <c r="B49" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="C49" s="116"/>
-      <c r="D49" s="113"/>
-      <c r="E49" s="117"/>
-      <c r="F49" s="117"/>
+      <c r="C49" s="94"/>
+      <c r="D49" s="91">
+        <v>1</v>
+      </c>
+      <c r="E49" s="95">
+        <v>44630</v>
+      </c>
+      <c r="F49" s="95">
+        <v>44641</v>
+      </c>
       <c r="G49" s="10"/>
-      <c r="H49" s="10" t="str">
+      <c r="H49" s="10">
         <f t="shared" si="40"/>
-        <v/>
+        <v>12</v>
       </c>
       <c r="I49" s="23"/>
       <c r="J49" s="23"/>
@@ -17022,17 +17067,23 @@
       <c r="JN49" s="67"/>
     </row>
     <row r="50" spans="2:274" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="116" t="s">
+      <c r="B50" s="94" t="s">
         <v>75</v>
       </c>
-      <c r="C50" s="116"/>
-      <c r="D50" s="113"/>
-      <c r="E50" s="117"/>
-      <c r="F50" s="117"/>
+      <c r="C50" s="94"/>
+      <c r="D50" s="91">
+        <v>1</v>
+      </c>
+      <c r="E50" s="95">
+        <v>44641</v>
+      </c>
+      <c r="F50" s="95">
+        <v>44648</v>
+      </c>
       <c r="G50" s="10"/>
-      <c r="H50" s="10" t="str">
+      <c r="H50" s="10">
         <f t="shared" si="40"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="I50" s="23"/>
       <c r="J50" s="23"/>
@@ -17302,17 +17353,23 @@
       <c r="JN50" s="67"/>
     </row>
     <row r="51" spans="2:274" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="116" t="s">
-        <v>62</v>
-      </c>
-      <c r="C51" s="116"/>
-      <c r="D51" s="113"/>
-      <c r="E51" s="117"/>
-      <c r="F51" s="117"/>
+      <c r="B51" s="94" t="s">
+        <v>63</v>
+      </c>
+      <c r="C51" s="94"/>
+      <c r="D51" s="91">
+        <v>1</v>
+      </c>
+      <c r="E51" s="95">
+        <v>44676</v>
+      </c>
+      <c r="F51" s="95">
+        <v>44690</v>
+      </c>
       <c r="G51" s="10"/>
-      <c r="H51" s="10" t="str">
+      <c r="H51" s="10">
         <f t="shared" si="40"/>
-        <v/>
+        <v>15</v>
       </c>
       <c r="I51" s="23"/>
       <c r="J51" s="23"/>
@@ -17582,13 +17639,15 @@
       <c r="JN51" s="67"/>
     </row>
     <row r="52" spans="2:274" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="116" t="s">
-        <v>63</v>
-      </c>
-      <c r="C52" s="116"/>
-      <c r="D52" s="113"/>
-      <c r="E52" s="117"/>
-      <c r="F52" s="117"/>
+      <c r="B52" s="96" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52" s="96"/>
+      <c r="D52" s="97"/>
+      <c r="E52" s="98">
+        <v>3</v>
+      </c>
+      <c r="F52" s="99"/>
       <c r="G52" s="10"/>
       <c r="H52" s="10" t="str">
         <f t="shared" si="40"/>
@@ -17862,17 +17921,23 @@
       <c r="JN52" s="67"/>
     </row>
     <row r="53" spans="2:274" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="118" t="s">
-        <v>67</v>
-      </c>
-      <c r="C53" s="118"/>
-      <c r="D53" s="119"/>
-      <c r="E53" s="120"/>
-      <c r="F53" s="121"/>
+      <c r="B53" s="100" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53" s="100"/>
+      <c r="D53" s="97">
+        <v>1</v>
+      </c>
+      <c r="E53" s="101">
+        <v>44536</v>
+      </c>
+      <c r="F53" s="101">
+        <v>44592</v>
+      </c>
       <c r="G53" s="10"/>
-      <c r="H53" s="10" t="str">
+      <c r="H53" s="10">
         <f t="shared" si="40"/>
-        <v/>
+        <v>57</v>
       </c>
       <c r="I53" s="23"/>
       <c r="J53" s="23"/>
@@ -18142,23 +18207,23 @@
       <c r="JN53" s="67"/>
     </row>
     <row r="54" spans="2:274" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="122" t="s">
-        <v>68</v>
-      </c>
-      <c r="C54" s="122"/>
-      <c r="D54" s="119">
+      <c r="B54" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" s="100"/>
+      <c r="D54" s="97">
         <v>1</v>
       </c>
-      <c r="E54" s="123">
-        <v>44536</v>
-      </c>
-      <c r="F54" s="123">
+      <c r="E54" s="101">
         <v>44592</v>
+      </c>
+      <c r="F54" s="101">
+        <v>44599</v>
       </c>
       <c r="G54" s="10"/>
       <c r="H54" s="10">
         <f t="shared" si="40"/>
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="I54" s="23"/>
       <c r="J54" s="23"/>
@@ -18428,23 +18493,17 @@
       <c r="JN54" s="67"/>
     </row>
     <row r="55" spans="2:274" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="122" t="s">
-        <v>69</v>
-      </c>
-      <c r="C55" s="122"/>
-      <c r="D55" s="119">
-        <v>1</v>
-      </c>
-      <c r="E55" s="123">
-        <v>44592</v>
-      </c>
-      <c r="F55" s="123">
-        <v>44599</v>
-      </c>
+      <c r="B55" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" s="72"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="52"/>
+      <c r="F55" s="53"/>
       <c r="G55" s="10"/>
-      <c r="H55" s="10">
+      <c r="H55" s="10" t="str">
         <f t="shared" si="40"/>
-        <v>8</v>
+        <v/>
       </c>
       <c r="I55" s="23"/>
       <c r="J55" s="23"/>
@@ -18714,17 +18773,23 @@
       <c r="JN55" s="67"/>
     </row>
     <row r="56" spans="2:274" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="72" t="s">
-        <v>32</v>
-      </c>
-      <c r="C56" s="72"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="52"/>
-      <c r="F56" s="53"/>
+      <c r="B56" s="71" t="s">
+        <v>33</v>
+      </c>
+      <c r="C56" s="71"/>
+      <c r="D56" s="18">
+        <v>1</v>
+      </c>
+      <c r="E56" s="59">
+        <v>44637</v>
+      </c>
+      <c r="F56" s="59">
+        <v>44637</v>
+      </c>
       <c r="G56" s="10"/>
-      <c r="H56" s="10" t="str">
+      <c r="H56" s="10">
         <f t="shared" ref="H56:H61" si="41">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I56" s="23"/>
       <c r="J56" s="23"/>
@@ -18995,20 +19060,22 @@
     </row>
     <row r="57" spans="2:274" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="71" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C57" s="71"/>
-      <c r="D57" s="18"/>
+      <c r="D57" s="18">
+        <v>1</v>
+      </c>
       <c r="E57" s="59">
-        <v>44637</v>
+        <v>44698</v>
       </c>
       <c r="F57" s="59">
-        <v>44637</v>
+        <v>44699</v>
       </c>
       <c r="G57" s="10"/>
       <c r="H57" s="10">
         <f t="shared" si="41"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I57" s="23"/>
       <c r="J57" s="23"/>
@@ -19279,12 +19346,14 @@
     </row>
     <row r="58" spans="2:274" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="71" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C58" s="71"/>
-      <c r="D58" s="18"/>
+      <c r="D58" s="18">
+        <v>1</v>
+      </c>
       <c r="E58" s="59">
-        <v>44698</v>
+        <v>44699</v>
       </c>
       <c r="F58" s="59">
         <v>44699</v>
@@ -19292,7 +19361,7 @@
       <c r="G58" s="10"/>
       <c r="H58" s="10">
         <f t="shared" si="41"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I58" s="23"/>
       <c r="J58" s="23"/>
@@ -19562,21 +19631,20 @@
       <c r="JN58" s="67"/>
     </row>
     <row r="59" spans="2:274" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="71" t="s">
-        <v>35</v>
-      </c>
-      <c r="C59" s="71"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="59">
-        <v>44699</v>
-      </c>
-      <c r="F59" s="59">
-        <v>44699</v>
+      <c r="B59" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="C59" s="44"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="60"/>
+      <c r="F59" s="70">
+        <f ca="1">F58 - TODAY()</f>
+        <v>-9</v>
       </c>
       <c r="G59" s="10"/>
-      <c r="H59" s="10">
-        <f t="shared" si="41"/>
-        <v>1</v>
+      <c r="H59" s="10" t="str">
+        <f t="shared" ca="1" si="41"/>
+        <v/>
       </c>
       <c r="I59" s="23"/>
       <c r="J59" s="23"/>
@@ -19846,19 +19914,16 @@
       <c r="JN59" s="67"/>
     </row>
     <row r="60" spans="2:274" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="C60" s="44"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="60"/>
-      <c r="F60" s="70">
-        <f ca="1">F59 - TODAY()</f>
-        <v>63</v>
-      </c>
+      <c r="B60" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C60" s="20"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="54"/>
+      <c r="F60" s="55"/>
       <c r="G60" s="10"/>
       <c r="H60" s="10" t="str">
-        <f t="shared" ca="1" si="41"/>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="I60" s="23"/>
@@ -20129,13 +20194,6 @@
       <c r="JN60" s="67"/>
     </row>
     <row r="61" spans="2:274" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C61" s="20"/>
-      <c r="D61" s="21"/>
-      <c r="E61" s="54"/>
-      <c r="F61" s="55"/>
       <c r="G61" s="22"/>
       <c r="H61" s="22" t="str">
         <f t="shared" si="41"/>
@@ -20410,55 +20468,12 @@
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="BF4:BL4"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="CV4:DB4"/>
-    <mergeCell ref="DC4:DI4"/>
-    <mergeCell ref="DJ4:DP4"/>
-    <mergeCell ref="DQ4:DW4"/>
-    <mergeCell ref="DX4:ED4"/>
-    <mergeCell ref="EE4:EK4"/>
-    <mergeCell ref="GI4:GO4"/>
-    <mergeCell ref="GP4:GV4"/>
-    <mergeCell ref="GW4:HC4"/>
-    <mergeCell ref="EL4:ER4"/>
-    <mergeCell ref="ES4:EY4"/>
-    <mergeCell ref="EZ4:FF4"/>
-    <mergeCell ref="FG4:FM4"/>
-    <mergeCell ref="FN4:FT4"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
     <mergeCell ref="JV4:KB4"/>
     <mergeCell ref="KC4:KI4"/>
     <mergeCell ref="KJ4:KP4"/>
@@ -20475,16 +20490,59 @@
     <mergeCell ref="IF4:IL4"/>
     <mergeCell ref="FU4:GA4"/>
     <mergeCell ref="GB4:GH4"/>
+    <mergeCell ref="GP4:GV4"/>
+    <mergeCell ref="GW4:HC4"/>
+    <mergeCell ref="EL4:ER4"/>
+    <mergeCell ref="ES4:EY4"/>
+    <mergeCell ref="EZ4:FF4"/>
+    <mergeCell ref="FG4:FM4"/>
+    <mergeCell ref="FN4:FT4"/>
+    <mergeCell ref="DJ4:DP4"/>
+    <mergeCell ref="DQ4:DW4"/>
+    <mergeCell ref="DX4:ED4"/>
+    <mergeCell ref="EE4:EK4"/>
+    <mergeCell ref="GI4:GO4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
+    <mergeCell ref="CV4:DB4"/>
+    <mergeCell ref="DC4:DI4"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="BT4:BZ4"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="AD4:AJ4"/>
   </mergeCells>
   <phoneticPr fontId="35" type="noConversion"/>
-  <conditionalFormatting sqref="D7:D61">
+  <conditionalFormatting sqref="D7:D60">
     <cfRule type="dataBar" priority="26">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -20557,7 +20615,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="60" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="14" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -20577,7 +20635,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D61</xm:sqref>
+          <xm:sqref>D7:D60</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>